<commit_message>
Updated memos for Cost Baseline Diagram, Risk Matrix, Monte Carlo
</commit_message>
<xml_diff>
--- a/templates/2.3_CostBaselineDiagramTemplate.xlsx
+++ b/templates/2.3_CostBaselineDiagramTemplate.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding Projects\PMI_CaseStudyChallenge\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57B10A1-E6FB-4AA8-B066-F4290D5A72BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BA7DEB-51F4-4A2C-AA77-91B71E74551C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Item Name</t>
   </si>
@@ -87,12 +87,162 @@
   </si>
   <si>
     <t>PaintTech EasyDry Paint Booth (Remaining)</t>
+  </si>
+  <si>
+    <t>2021 Cost Table</t>
+  </si>
+  <si>
+    <t>Module 2.3 - Visualizing the Budget - Instructions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Revise the 2021 cost table with the new line items and amounts.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Review the memos to identify updated costs, removed tasks, and any new requirements.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Assign costs to the appropriate dates based on your Gantt chart (e.g., deposits, permits, delivery, installation).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Update the cumulative totals in the table.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Create an updated Cost Baseline Diagram (cumulative cost curve) from your table.</t>
+    </r>
+  </si>
+  <si>
+    <t>For tasks with ongoing costs (e.g., rentals, prep, installation), try spreading the total evenly across their duration instead of recording as a single lump sum.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">7. (Bonus): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Simplify the visual, highlight the key cost changes from 2021, and apply formatting that guides the viewer’s attention.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,15 +260,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFCF3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -276,44 +450,326 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFCF3"/>
+      <color rgb="FFFFFFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -380,7 +836,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$E$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -403,7 +859,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$15</c:f>
+              <c:f>Sheet1!$C$14:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
@@ -454,9 +910,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$15</c:f>
+              <c:f>Sheet1!$E$14:$E$27</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>"$"#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -593,7 +1049,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -646,10 +1102,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1233,16 +1686,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>743108</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>22952</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19208</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>13427</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>224839</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>17235</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>253414</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>7710</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1273,7 +1726,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1281,34 +1734,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office 2007 - 2010">
@@ -1557,311 +2010,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D2ADAA-E5CD-4779-AF10-AA9BBEDB0BE3}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="25"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="25"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="25"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
+    </row>
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="28"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E13" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="14">
+      <c r="C14" s="11">
         <v>44315</v>
       </c>
-      <c r="C2" s="10">
+      <c r="D14" s="14">
         <v>0</v>
       </c>
-      <c r="D2" s="6">
+      <c r="E14" s="15">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="15">
+      <c r="C15" s="12">
         <v>44336</v>
       </c>
-      <c r="C3" s="11">
+      <c r="D15" s="16">
         <v>25000</v>
       </c>
-      <c r="D3" s="7">
-        <f>D2+C3</f>
+      <c r="E15" s="17">
+        <f>E14+D15</f>
         <v>25000</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15">
+      <c r="C16" s="12">
         <v>44343</v>
       </c>
-      <c r="C4" s="11">
+      <c r="D16" s="16">
         <v>1500</v>
       </c>
-      <c r="D4" s="7">
-        <f t="shared" ref="D4:D15" si="0">D3+C4</f>
+      <c r="E16" s="17">
+        <f t="shared" ref="E16:E27" si="0">E15+D16</f>
         <v>26500</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15">
+      <c r="C17" s="12">
         <v>44343</v>
       </c>
-      <c r="C5" s="11">
+      <c r="D17" s="16">
         <v>5000</v>
       </c>
-      <c r="D5" s="7">
+      <c r="E17" s="17">
         <f t="shared" si="0"/>
         <v>31500</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="15">
+      <c r="C18" s="12">
         <v>44361</v>
       </c>
-      <c r="C6" s="11">
+      <c r="D18" s="16">
         <v>500</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E18" s="17">
         <f t="shared" si="0"/>
         <v>32000</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="15">
+      <c r="C19" s="12">
         <v>44361</v>
       </c>
-      <c r="C7" s="11">
+      <c r="D19" s="16">
         <v>150</v>
       </c>
-      <c r="D7" s="7">
+      <c r="E19" s="17">
         <f t="shared" si="0"/>
         <v>32150</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15">
+      <c r="C20" s="12">
         <v>44361</v>
       </c>
-      <c r="C8" s="11">
+      <c r="D20" s="16">
         <v>150</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E20" s="17">
         <f t="shared" si="0"/>
         <v>32300</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="15">
+      <c r="C21" s="12">
         <v>44361</v>
       </c>
-      <c r="C9" s="11">
+      <c r="D21" s="16">
         <v>150</v>
       </c>
-      <c r="D9" s="7">
+      <c r="E21" s="17">
         <f t="shared" si="0"/>
         <v>32450</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="15">
+      <c r="C22" s="12">
         <v>44361</v>
       </c>
-      <c r="C10" s="11">
+      <c r="D22" s="16">
         <v>1000</v>
       </c>
-      <c r="D10" s="7">
+      <c r="E22" s="17">
         <f t="shared" si="0"/>
         <v>33450</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="15">
+      <c r="C23" s="12">
         <v>44361</v>
       </c>
-      <c r="C11" s="11">
+      <c r="D23" s="16">
         <v>1400</v>
       </c>
-      <c r="D11" s="7">
+      <c r="E23" s="17">
         <f t="shared" si="0"/>
         <v>34850</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="15">
+      <c r="C24" s="12">
         <v>44361</v>
       </c>
-      <c r="C12" s="11">
+      <c r="D24" s="16">
         <v>1200</v>
       </c>
-      <c r="D12" s="7">
+      <c r="E24" s="17">
         <f t="shared" si="0"/>
         <v>36050</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="15">
+      <c r="C25" s="12">
         <v>44366</v>
       </c>
-      <c r="C13" s="11">
+      <c r="D25" s="16">
         <v>25000</v>
       </c>
-      <c r="D13" s="7">
+      <c r="E25" s="17">
         <f t="shared" si="0"/>
         <v>61050</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="15">
+      <c r="C26" s="12">
         <v>44367</v>
       </c>
-      <c r="C14" s="11">
+      <c r="D26" s="16">
         <v>1500</v>
       </c>
-      <c r="D14" s="7">
+      <c r="E26" s="17">
         <f t="shared" si="0"/>
         <v>62550</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+    </row>
+    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="16">
+      <c r="C27" s="13">
         <v>44369</v>
       </c>
-      <c r="C15" s="12">
+      <c r="D27" s="18">
         <v>5000</v>
       </c>
-      <c r="D15" s="8">
+      <c r="E27" s="19">
         <f t="shared" si="0"/>
         <v>67550</v>
       </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B5:L5"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="B9:L9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated memos 1,7. Updated cost baseline diagram template, updated WBS section to clarify draw.io
</commit_message>
<xml_diff>
--- a/templates/2.3_CostBaselineDiagramTemplate.xlsx
+++ b/templates/2.3_CostBaselineDiagramTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding Projects\PMI_CaseStudyChallenge\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BA7DEB-51F4-4A2C-AA77-91B71E74551C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB42903A-2D03-4044-B654-43B26F5DABEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Cumulative Cost</t>
   </si>
   <si>
-    <t>Facility Inspection Fee</t>
-  </si>
-  <si>
     <t>LADBS Building Permit</t>
   </si>
   <si>
@@ -66,15 +63,6 @@
   </si>
   <si>
     <t>SCAQMD Permit to Operate</t>
-  </si>
-  <si>
-    <t>Facility Prep (Electrical, HVAC)</t>
-  </si>
-  <si>
-    <t>Equipment rentals (Boom lift, etc.)</t>
-  </si>
-  <si>
-    <t>Installation (Sprinklers, etc.)</t>
   </si>
   <si>
     <t>Project Start</t>
@@ -210,7 +198,19 @@
     </r>
   </si>
   <si>
-    <t>For tasks with ongoing costs (e.g., rentals, prep, installation), try spreading the total evenly across their duration instead of recording as a single lump sum.</t>
+    <t>Facility Inspection Fees</t>
+  </si>
+  <si>
+    <t>Sprinkler installation</t>
+  </si>
+  <si>
+    <t>Facility Prep (Electrical, HVAC)</t>
+  </si>
+  <si>
+    <t>Equipment rentals (Boom lift, etc.)</t>
+  </si>
+  <si>
+    <t>For tasks with ongoing costs (e.g., rentals, facility prep), spread the total cost evenly across their duration instead of recording it as a single lump sum at the beginning of the task</t>
   </si>
   <si>
     <r>
@@ -222,7 +222,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">7. (Bonus): </t>
+      <t xml:space="preserve">7. (Bonus) </t>
     </r>
     <r>
       <rPr>
@@ -232,7 +232,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Simplify the visual, highlight the key cost changes from 2021, and apply formatting that guides the viewer’s attention.</t>
+      <t>Improve the diagram, highlight the key cost changes from 2021, and apply formatting that guides the viewer’s attention.</t>
     </r>
   </si>
 </sst>
@@ -241,7 +241,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -292,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -312,105 +312,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -423,31 +330,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -665,98 +548,134 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -864,46 +783,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44315</c:v>
+                  <c:v>44237</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44336</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44343</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44343</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44361</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44361</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44361</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44361</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44361</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44361</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44361</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44366</c:v>
+                  <c:v>44254</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44367</c:v>
+                  <c:v>44283</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44369</c:v>
+                  <c:v>44289</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -912,7 +831,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$14:$E$27</c:f>
               <c:numCache>
-                <c:formatCode>"$"#,##0</c:formatCode>
+                <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -924,31 +843,31 @@
                   <c:v>26500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31500</c:v>
+                  <c:v>27000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32000</c:v>
+                  <c:v>27150</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32150</c:v>
+                  <c:v>27300</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32300</c:v>
+                  <c:v>27450</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32450</c:v>
+                  <c:v>28450</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33450</c:v>
+                  <c:v>29850</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34850</c:v>
+                  <c:v>31050</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36050</c:v>
+                  <c:v>33550</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>61050</c:v>
+                  <c:v>33850</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>62550</c:v>
@@ -1049,7 +968,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1687,15 +1606,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>19208</xdr:colOff>
+      <xdr:colOff>19209</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>13427</xdr:rowOff>
+      <xdr:rowOff>32477</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>253414</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>7710</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2010,142 +1929,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D2ADAA-E5CD-4779-AF10-AA9BBEDB0BE3}">
-  <dimension ref="B1:L28"/>
+  <dimension ref="B1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="30"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="33"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="22"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="33"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="25"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="25"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="25"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="25"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="33"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="33"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="28"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="36"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F10" s="1"/>
@@ -2154,250 +2073,338 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
+      <c r="B12" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="11">
-        <v>44315</v>
-      </c>
-      <c r="D14" s="14">
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="8">
+        <v>44237</v>
+      </c>
+      <c r="D14" s="9">
         <v>0</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="10">
         <v>0</v>
       </c>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="12">
-        <v>44336</v>
-      </c>
-      <c r="D15" s="16">
+      <c r="B15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="11">
+        <v>44254</v>
+      </c>
+      <c r="D15" s="12">
         <v>25000</v>
       </c>
-      <c r="E15" s="17">
-        <f>E14+D15</f>
+      <c r="E15" s="13">
         <v>25000</v>
       </c>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="11">
+        <v>44254</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1500</v>
+      </c>
+      <c r="E16" s="13">
+        <v>26500</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="12">
-        <v>44343</v>
-      </c>
-      <c r="D16" s="16">
+      <c r="C17" s="11">
+        <v>44254</v>
+      </c>
+      <c r="D17" s="12">
+        <v>500</v>
+      </c>
+      <c r="E17" s="13">
+        <v>27000</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="11">
+        <v>44254</v>
+      </c>
+      <c r="D18" s="12">
+        <v>150</v>
+      </c>
+      <c r="E18" s="13">
+        <v>27150</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="11">
+        <v>44254</v>
+      </c>
+      <c r="D19" s="12">
+        <v>150</v>
+      </c>
+      <c r="E19" s="13">
+        <v>27300</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="11">
+        <v>44254</v>
+      </c>
+      <c r="D20" s="12">
+        <v>150</v>
+      </c>
+      <c r="E20" s="13">
+        <v>27450</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="11">
+        <v>44254</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="13">
+        <v>28450</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="11">
+        <v>44254</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1400</v>
+      </c>
+      <c r="E22" s="13">
+        <v>29850</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="11">
+        <v>44254</v>
+      </c>
+      <c r="D23" s="12">
+        <v>1200</v>
+      </c>
+      <c r="E23" s="13">
+        <v>31050</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="41">
+        <v>44254</v>
+      </c>
+      <c r="D24" s="42">
+        <v>5000</v>
+      </c>
+      <c r="E24" s="43">
+        <v>33550</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="41">
+        <v>44254</v>
+      </c>
+      <c r="D25" s="42">
         <v>1500</v>
       </c>
-      <c r="E16" s="17">
-        <f t="shared" ref="E16:E27" si="0">E15+D16</f>
-        <v>26500</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="12">
-        <v>44343</v>
-      </c>
-      <c r="D17" s="16">
-        <v>5000</v>
-      </c>
-      <c r="E17" s="17">
-        <f t="shared" si="0"/>
-        <v>31500</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="12">
-        <v>44361</v>
-      </c>
-      <c r="D18" s="16">
-        <v>500</v>
-      </c>
-      <c r="E18" s="17">
-        <f t="shared" si="0"/>
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="12">
-        <v>44361</v>
-      </c>
-      <c r="D19" s="16">
-        <v>150</v>
-      </c>
-      <c r="E19" s="17">
-        <f t="shared" si="0"/>
-        <v>32150</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="12">
-        <v>44361</v>
-      </c>
-      <c r="D20" s="16">
-        <v>150</v>
-      </c>
-      <c r="E20" s="17">
-        <f t="shared" si="0"/>
-        <v>32300</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="12">
-        <v>44361</v>
-      </c>
-      <c r="D21" s="16">
-        <v>150</v>
-      </c>
-      <c r="E21" s="17">
-        <f t="shared" si="0"/>
-        <v>32450</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="12">
-        <v>44361</v>
-      </c>
-      <c r="D22" s="16">
-        <v>1000</v>
-      </c>
-      <c r="E22" s="17">
-        <f t="shared" si="0"/>
-        <v>33450</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="12">
-        <v>44361</v>
-      </c>
-      <c r="D23" s="16">
-        <v>1400</v>
-      </c>
-      <c r="E23" s="17">
-        <f t="shared" si="0"/>
-        <v>34850</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="12">
-        <v>44361</v>
-      </c>
-      <c r="D24" s="16">
-        <v>1200</v>
-      </c>
-      <c r="E24" s="17">
-        <f t="shared" si="0"/>
-        <v>36050</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="12">
-        <v>44366</v>
-      </c>
-      <c r="D25" s="16">
+      <c r="E25" s="43">
+        <v>33850</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="14">
+        <v>44283</v>
+      </c>
+      <c r="D26" s="15">
         <v>25000</v>
       </c>
-      <c r="E25" s="17">
-        <f t="shared" si="0"/>
-        <v>61050</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="12">
-        <v>44367</v>
-      </c>
-      <c r="D26" s="16">
-        <v>1500</v>
-      </c>
-      <c r="E26" s="17">
-        <f t="shared" si="0"/>
+      <c r="E26" s="16">
         <v>62550</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="13">
-        <v>44369</v>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="17">
+        <v>44289</v>
       </c>
       <c r="D27" s="18">
         <v>5000</v>
       </c>
       <c r="E27" s="19">
-        <f t="shared" si="0"/>
         <v>67550</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="22"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="22"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="22"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="22"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="22"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="22"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="22"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="22"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="22"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="22"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="B9:L9"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B4:L4"/>
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="B6:L6"/>
     <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
updated cost baseline template
</commit_message>
<xml_diff>
--- a/templates/2.3_CostBaselineDiagramTemplate.xlsx
+++ b/templates/2.3_CostBaselineDiagramTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding Projects\PMI_CaseStudyChallenge\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB42903A-2D03-4044-B654-43B26F5DABEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C4538B-06C3-4D00-87BF-602FCFF649FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Item Name</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>PaintTech EasyDry Paint Booth (Deposit)</t>
-  </si>
-  <si>
-    <t>PaintTech EasyDry Paint Booth (Remaining)</t>
   </si>
   <si>
     <t>2021 Cost Table</t>
@@ -235,13 +232,20 @@
       <t>Improve the diagram, highlight the key cost changes from 2021, and apply formatting that guides the viewer’s attention.</t>
     </r>
   </si>
+  <si>
+    <t>Paint Booth installation</t>
+  </si>
+  <si>
+    <t>PaintTech EasyDry Paint Booth (Remaining upon delivery)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -548,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,39 +576,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -665,16 +645,37 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -778,10 +779,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$14:$C$27</c:f>
+              <c:f>Sheet1!$C$14:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>44237</c:v>
                 </c:pt>
@@ -822,6 +823,9 @@
                   <c:v>44283</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>44284</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>44289</c:v>
                 </c:pt>
               </c:numCache>
@@ -829,10 +833,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$14:$E$27</c:f>
+              <c:f>Sheet1!$E$14:$E$28</c:f>
               <c:numCache>
-                <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:formatCode>"$"#,##0</c:formatCode>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -864,16 +868,19 @@
                   <c:v>31050</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33550</c:v>
+                  <c:v>36050</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33850</c:v>
+                  <c:v>37550</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>62550</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>67550</c:v>
+                  <c:v>64550</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>69550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -968,7 +975,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)" sourceLinked="1"/>
+        <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1929,158 +1936,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D2ADAA-E5CD-4779-AF10-AA9BBEDB0BE3}">
-  <dimension ref="B1:L44"/>
+  <dimension ref="B1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:L9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="12" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="19"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="25"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="30"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="33"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="33"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="25"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="33"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="33"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="33"/>
-    </row>
-    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="34" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="25"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
+    </row>
+    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="28"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-    </row>
-    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="31"/>
+    </row>
+    <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
@@ -2094,305 +2100,350 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="8">
         <v>44237</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="32">
         <v>0</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="33">
         <v>0</v>
       </c>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="9">
         <v>44254</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="34">
         <v>25000</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="35">
+        <f>E14+D15</f>
         <v>25000</v>
       </c>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="11">
+        <v>20</v>
+      </c>
+      <c r="C16" s="9">
         <v>44254</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="34">
         <v>1500</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="35">
+        <f t="shared" ref="E16:E28" si="0">E15+D16</f>
         <v>26500</v>
       </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="9">
         <v>44254</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="34">
         <v>500</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="35">
+        <f t="shared" si="0"/>
         <v>27000</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="9">
         <v>44254</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="34">
         <v>150</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="35">
+        <f t="shared" si="0"/>
         <v>27150</v>
       </c>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="9">
         <v>44254</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="34">
         <v>150</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="35">
+        <f t="shared" si="0"/>
         <v>27300</v>
       </c>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="9">
         <v>44254</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="34">
         <v>150</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="35">
+        <f t="shared" si="0"/>
         <v>27450</v>
       </c>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="9">
         <v>44254</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="34">
         <v>1000</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="35">
+        <f t="shared" si="0"/>
         <v>28450</v>
       </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="9">
         <v>44254</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="34">
         <v>1400</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="35">
+        <f t="shared" si="0"/>
         <v>29850</v>
       </c>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="9">
         <v>44254</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="34">
         <v>1200</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="35">
+        <f t="shared" si="0"/>
         <v>31050</v>
       </c>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="40" t="s">
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="40">
+        <v>44254</v>
+      </c>
+      <c r="D24" s="41">
+        <v>5000</v>
+      </c>
+      <c r="E24" s="42">
+        <f t="shared" si="0"/>
+        <v>36050</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C25" s="40">
         <v>44254</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D25" s="41">
+        <v>1500</v>
+      </c>
+      <c r="E25" s="42">
+        <f t="shared" si="0"/>
+        <v>37550</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="10">
+        <v>44283</v>
+      </c>
+      <c r="D26" s="36">
+        <v>25000</v>
+      </c>
+      <c r="E26" s="35">
+        <f t="shared" si="0"/>
+        <v>62550</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="10">
+        <v>44284</v>
+      </c>
+      <c r="D27" s="36">
+        <v>2000</v>
+      </c>
+      <c r="E27" s="35">
+        <f t="shared" si="0"/>
+        <v>64550</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="11">
+        <v>44289</v>
+      </c>
+      <c r="D28" s="37">
         <v>5000</v>
       </c>
-      <c r="E24" s="43">
-        <v>33550</v>
-      </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="41">
-        <v>44254</v>
-      </c>
-      <c r="D25" s="42">
-        <v>1500</v>
-      </c>
-      <c r="E25" s="43">
-        <v>33850</v>
-      </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="14">
-        <v>44283</v>
-      </c>
-      <c r="D26" s="15">
-        <v>25000</v>
-      </c>
-      <c r="E26" s="16">
-        <v>62550</v>
-      </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="17">
-        <v>44289</v>
-      </c>
-      <c r="D27" s="18">
-        <v>5000</v>
-      </c>
-      <c r="E27" s="19">
-        <v>67550</v>
-      </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="22"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
+      <c r="E28" s="39">
+        <f t="shared" si="0"/>
+        <v>69550</v>
+      </c>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="22"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="22"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="22"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="22"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="22"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="22"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="22"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="22"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="22"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="22"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>